<commit_message>
Added cl interpolation along the span
</commit_message>
<xml_diff>
--- a/initialization/Aircraft.xlsx
+++ b/initialization/Aircraft.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claum\OneDrive\Desktop\TesiMagistrale\tesi-magistrale-claudio-mirabella\initialization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5733CC8-6BEE-484B-8157-6FED32DF692C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{71EF77EE-0D1D-4A19-82F6-696BF66C8AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1059,187 +1059,187 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>34</v>
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>2.589</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>19</v>
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21">
+        <v>5.2</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22">
+        <v>10.446</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>40</v>
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B24">
-        <v>2.589</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>42</v>
+        <v>2.8839999999999999</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>43</v>
+      <c r="A25" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B25">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>45</v>
+      <c r="A26" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="B26">
-        <v>10.446</v>
+        <v>0.33</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>46</v>
+      <c r="A27" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B27">
-        <v>100</v>
+        <v>0.25</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>48</v>
+      <c r="A28" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="B28">
-        <v>2.8839999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="6" t="s">
-        <v>49</v>
+      <c r="A29" t="s">
+        <v>51</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B30">
-        <v>0.33</v>
+        <v>1.492</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="6" t="s">
-        <v>69</v>
+      <c r="A31" t="s">
+        <v>53</v>
       </c>
       <c r="B31">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="6" t="s">
-        <v>70</v>
+      <c r="A32" t="s">
+        <v>54</v>
       </c>
       <c r="B32">
-        <v>0.25</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>51</v>
+      <c r="A33" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B33">
-        <v>0.52900000000000003</v>
+        <v>2.8839999999999999</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B34">
-        <v>1.492</v>
+        <v>0</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>53</v>
+      <c r="A35" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>54</v>
+      <c r="A36" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="B36">
-        <v>4.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>19</v>
@@ -1247,231 +1247,231 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37">
-        <v>2.8839999999999999</v>
+        <v>59</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0.8</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="10">
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39">
-        <v>0.33</v>
+        <v>61</v>
+      </c>
+      <c r="B39" s="10">
+        <v>0.36499999999999999</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40">
-        <v>0.05</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="10">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="10">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B40" s="10">
         <f>[1]Aircraft!$K$24</f>
         <v>0.82195210959999987</v>
       </c>
+      <c r="C40" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42">
+        <v>-2.18378662E-2</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43">
+        <v>0.43606477249999998</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44">
+        <v>-0.56312854999999995</v>
+      </c>
       <c r="C44" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="10">
-        <v>1.5</v>
+      <c r="A45" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45">
+        <v>-0.261519</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="10" t="s">
-        <v>64</v>
+      <c r="A46" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="B46">
-        <v>-2.18378662E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="10" t="s">
-        <v>65</v>
+      <c r="A47" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="B47">
-        <v>0.43606477249999998</v>
+        <v>0</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="10" t="s">
-        <v>66</v>
+      <c r="A48" t="s">
+        <v>72</v>
       </c>
       <c r="B48">
-        <v>-0.56312854999999995</v>
+        <v>0</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="6" t="s">
-        <v>67</v>
+      <c r="A49" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B49">
-        <v>-0.261519</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>19</v>
+        <v>0.498</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="11" t="s">
-        <v>68</v>
+      <c r="A50" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="B50">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>19</v>
+        <v>0.498</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="6" t="s">
-        <v>71</v>
+      <c r="A51" t="s">
+        <v>75</v>
       </c>
       <c r="B51">
-        <v>0</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>44</v>
+        <v>3</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B52">
-        <v>0</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>19</v>
+        <v>0.14069999999999999</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="4" t="s">
-        <v>73</v>
+      <c r="A53" t="s">
+        <v>79</v>
       </c>
       <c r="B53">
-        <v>0.498</v>
-      </c>
-      <c r="C53" s="1" t="s">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="4" t="s">
-        <v>74</v>
+      <c r="A54" t="s">
+        <v>80</v>
       </c>
       <c r="B54">
-        <v>0.498</v>
-      </c>
-      <c r="C54" s="1" t="s">
+        <v>0.154</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>1.9E-2</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B56">
-        <v>0.14069999999999999</v>
+        <v>1.63</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B57">
-        <v>0.90800000000000003</v>
+        <v>2.5379999999999998</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>20</v>
@@ -1479,98 +1479,98 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B58">
-        <v>0.154</v>
+        <v>0.627</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B59">
-        <v>1.9E-2</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" t="s">
-        <v>82</v>
+      <c r="A60" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="B60">
-        <v>1.63</v>
+        <v>9.1300000000000006E-2</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B61">
-        <v>2.5379999999999998</v>
+        <v>3.64</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B62">
-        <v>0.627</v>
+        <v>0.42</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B63">
-        <v>0.97599999999999998</v>
+        <v>0.6</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="4" t="s">
-        <v>87</v>
+      <c r="A64" t="s">
+        <v>92</v>
       </c>
       <c r="B64">
-        <v>9.1300000000000006E-2</v>
+        <v>0.15</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B65">
-        <v>3.64</v>
+        <v>0.18</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B66">
-        <v>0.42</v>
+        <v>1.6379999999999999</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>44</v>
@@ -1578,131 +1578,132 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B67">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B68">
-        <v>0.15</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B69">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B70">
-        <v>1.6379999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B72">
-        <v>0.16500000000000001</v>
+        <v>0</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B74">
-        <v>0.2</v>
+        <v>1.49</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B75">
-        <v>0.12</v>
+        <f>B66+B74</f>
+        <v>3.1280000000000001</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B77">
-        <v>0.25</v>
+        <v>0.748</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B78">
-        <v>1.49</v>
+        <v>0.31359999999999999</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>44</v>
@@ -1710,77 +1711,76 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B79">
-        <f>B70+B78</f>
-        <v>3.1280000000000001</v>
+        <v>0.39290000000000003</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B80">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B81">
-        <v>0.748</v>
+        <v>0</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B82">
-        <v>0.31359999999999999</v>
+        <v>1</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B83">
-        <v>0.39290000000000003</v>
+        <v>0</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B84">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>99</v>
@@ -1788,10 +1788,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>99</v>
@@ -1799,32 +1799,32 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B88">
         <v>0</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>99</v>
@@ -1832,10 +1832,10 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B90">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>99</v>
@@ -1843,57 +1843,57 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B91">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>120</v>
-      </c>
-      <c r="B92">
-        <v>0</v>
-      </c>
-      <c r="C92" s="2" t="s">
+      <c r="A92" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C92" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" t="s">
-        <v>121</v>
-      </c>
-      <c r="B93">
-        <v>0</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>99</v>
+      <c r="A93" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>123</v>
-      </c>
-      <c r="B94">
-        <v>0</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>99</v>
+      <c r="A94" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>122</v>
-      </c>
-      <c r="B95">
-        <v>0</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>34</v>
+      <c r="A95" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1912,6 +1912,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100018B9E05534DD346B4DB939BB590FD48" ma:contentTypeVersion="6" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8afdbf8cd4174fbe595e5fb01abe9bda">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="90b0c0e5-2a5e-433a-b810-f67928ad9d5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30426a273519c332a31754524c74ef77" ns2:_="">
     <xsd:import namespace="90b0c0e5-2a5e-433a-b810-f67928ad9d5b"/>
@@ -2069,12 +2075,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F18F82C4-45FA-403F-BA0D-FD5B535E5FD9}">
   <ds:schemaRefs>
@@ -2084,6 +2084,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{105D9D7B-DF78-4314-955A-9D0D31EED297}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC2AD5F-F27B-4C05-A0BD-369CF16269A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2099,13 +2108,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{105D9D7B-DF78-4314-955A-9D0D31EED297}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correction of the lift curve model diagram; now all the points have the correct wing-body value of lift and alpha
</commit_message>
<xml_diff>
--- a/initialization/Aircraft.xlsx
+++ b/initialization/Aircraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claum\OneDrive\Desktop\TesiMagistrale\tesi-magistrale-claudio-mirabella\initialization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCB92392-8918-4579-85FB-087D1891D86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53346063-44A1-4350-A8DC-ED78291E49C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1912,6 +1912,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100018B9E05534DD346B4DB939BB590FD48" ma:contentTypeVersion="6" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8afdbf8cd4174fbe595e5fb01abe9bda">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="90b0c0e5-2a5e-433a-b810-f67928ad9d5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30426a273519c332a31754524c74ef77" ns2:_="">
     <xsd:import namespace="90b0c0e5-2a5e-433a-b810-f67928ad9d5b"/>
@@ -2069,12 +2075,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F18F82C4-45FA-403F-BA0D-FD5B535E5FD9}">
   <ds:schemaRefs>
@@ -2084,6 +2084,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{105D9D7B-DF78-4314-955A-9D0D31EED297}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC2AD5F-F27B-4C05-A0BD-369CF16269A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2099,13 +2108,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{105D9D7B-DF78-4314-955A-9D0D31EED297}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: now Schrenk's method is available
</commit_message>
<xml_diff>
--- a/initialization/Aircraft.xlsx
+++ b/initialization/Aircraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claum\OneDrive\Desktop\TesiMagistrale\tesi-magistrale-claudio-mirabella\initialization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04F3BB20-9237-424F-9740-54EBAD9FE436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB011CE8-664A-483C-9B98-D7EA27DBFDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,7 +393,7 @@
     <t>Airloads_flag</t>
   </si>
   <si>
-    <t>OPEN VSP</t>
+    <t>SCHRENK</t>
   </si>
 </sst>
 </file>
@@ -827,7 +827,7 @@
   <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1864,12 +1864,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100018B9E05534DD346B4DB939BB590FD48" ma:contentTypeVersion="6" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8afdbf8cd4174fbe595e5fb01abe9bda">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="90b0c0e5-2a5e-433a-b810-f67928ad9d5b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30426a273519c332a31754524c74ef77" ns2:_="">
     <xsd:import namespace="90b0c0e5-2a5e-433a-b810-f67928ad9d5b"/>
@@ -2027,6 +2021,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F18F82C4-45FA-403F-BA0D-FD5B535E5FD9}">
   <ds:schemaRefs>
@@ -2036,15 +2036,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{105D9D7B-DF78-4314-955A-9D0D31EED297}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC2AD5F-F27B-4C05-A0BD-369CF16269A2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2060,4 +2051,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{105D9D7B-DF78-4314-955A-9D0D31EED297}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update: hinge calculation for elevator and rudder plus engine loads stored correctly inside the structure variable
</commit_message>
<xml_diff>
--- a/initialization/Aircraft.xlsx
+++ b/initialization/Aircraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claum\OneDrive\Desktop\TesiMagistrale\tesi-magistrale-claudio-mirabella\initialization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08B12D75-251F-49F0-90A0-60EA5782B3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54197FCC-3681-4D17-A888-4EB45E5DF597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="166">
   <si>
     <t>field</t>
   </si>
@@ -502,6 +502,36 @@
   </si>
   <si>
     <t>Chalfaelevator</t>
+  </si>
+  <si>
+    <t>S_vertical</t>
+  </si>
+  <si>
+    <t>chord_vertical</t>
+  </si>
+  <si>
+    <t>S_rudder</t>
+  </si>
+  <si>
+    <t>chord_rudder</t>
+  </si>
+  <si>
+    <t>chord_ratio_rudder_cf_c</t>
+  </si>
+  <si>
+    <t>overhang_rudder</t>
+  </si>
+  <si>
+    <t>span_ratio_rudder</t>
+  </si>
+  <si>
+    <t>max_deflection_rudder</t>
+  </si>
+  <si>
+    <t>Chdeltarudder</t>
+  </si>
+  <si>
+    <t>Chalfarudder</t>
   </si>
 </sst>
 </file>
@@ -932,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1962,7 +1992,7 @@
         <v>119</v>
       </c>
       <c r="B93">
-        <v>73.5</v>
+        <v>11.185499999999999</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>120</v>
@@ -1984,7 +2014,7 @@
         <v>123</v>
       </c>
       <c r="B95">
-        <v>69</v>
+        <v>9.3212480000000006</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>120</v>
@@ -2047,7 +2077,7 @@
         <v>132</v>
       </c>
       <c r="B101">
-        <v>3.8</v>
+        <v>1.4</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>43</v>
@@ -2058,7 +2088,7 @@
         <v>133</v>
       </c>
       <c r="B102">
-        <v>76.7</v>
+        <v>18.5</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>43</v>
@@ -2069,7 +2099,7 @@
         <v>134</v>
       </c>
       <c r="B103">
-        <v>12.5</v>
+        <v>4.5</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>43</v>
@@ -2256,6 +2286,116 @@
         <v>-0.26900000000000002</v>
       </c>
       <c r="C120" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B121">
+        <v>0.1022</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B122">
+        <v>0.31359999999999999</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B123">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B124">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B125">
+        <v>0.35</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B126">
+        <v>0.12</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B127">
+        <v>0.8</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B128">
+        <v>25</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B129">
+        <v>-0.45379999999999998</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B130">
+        <v>-2.3999999999999998E-3</v>
+      </c>
+      <c r="C130" s="7" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>